<commit_message>
Replaced IRI problem by a provenance problem :-)
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/myvocab.xlsx
+++ b/inbox-excel-vocabs/myvocab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-dalito\voc4cat-template\inbox-excel-vocabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E62C96-CBD0-43AA-A4A2-2C8D4928974C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84552790-143F-458C-ACA9-79BBA1377DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="15825" tabRatio="652" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="173">
   <si>
     <t>Template version</t>
   </si>
@@ -652,7 +652,7 @@
     <t>0000-0001-2345-6789 Added item</t>
   </si>
   <si>
-    <t>https://example.org/ca10</t>
+    <t>https://example.org/c10</t>
   </si>
 </sst>
 </file>
@@ -6379,9 +6379,7 @@
       <c r="D3" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>171</v>
-      </c>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>

</xml_diff>

<commit_message>
Change vocab to state that should validate
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/myvocab.xlsx
+++ b/inbox-excel-vocabs/myvocab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-dalito\voc4cat-template\inbox-excel-vocabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84552790-143F-458C-ACA9-79BBA1377DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20E856F-B74C-4884-A7C1-B4637F77BE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="15825" tabRatio="652" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="15825" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="173">
   <si>
     <t>Template version</t>
   </si>
@@ -4301,7 +4301,7 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -6331,8 +6331,8 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6379,7 +6379,9 @@
       <c r="D3" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>

</xml_diff>